<commit_message>
Minor changes to README to improve formatting. Minor addition to database, which is still woefully inadequate.
</commit_message>
<xml_diff>
--- a/data-raw/database.xlsx
+++ b/data-raw/database.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>argument</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>R can't find your file. It may be looking in the wrong place (is your path correct?), may be looking for the wrong file (did you spell the name correctly?) or the file may be the wrong file type (a common one for me is trying to open .xls as a .xlsx and vice versa).</t>
+  </si>
+  <si>
+    <t>Error: Don't know how to add RHS to a theme object</t>
+  </si>
+  <si>
+    <t>Error: Don't know how to add RHS to an 'x' object</t>
+  </si>
+  <si>
+    <t>Common in ggplot2 errors: are you trying to add a layer, but forgot a plus sign  at the end of the line somewhere?</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -554,6 +563,17 @@
       </c>
       <c r="C6" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated database and interface.
</commit_message>
<xml_diff>
--- a/data-raw/database.xlsx
+++ b/data-raw/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24640" windowHeight="13100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24640" windowHeight="13100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="helpError" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="229">
   <si>
     <t>argument</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Error Message</t>
   </si>
   <si>
-    <t>Common Form</t>
-  </si>
-  <si>
     <t>Word</t>
   </si>
   <si>
@@ -144,13 +141,691 @@
   </si>
   <si>
     <t>Common in ggplot2 errors: are you trying to add a layer, but forgot a plus sign  at the end of the line somewhere?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0 (non-NA) cases</t>
+  </si>
+  <si>
+    <t>Error in lm.fit(x, y, offset = offset, singular.ok = singular.ok, ...) :   0 (non-NA) cases</t>
+  </si>
+  <si>
+    <t>All the data is missing and the function is wondering why you called it…!</t>
+  </si>
+  <si>
+    <t>In nnetar(pick) : Missing values in x, omitting rows</t>
+  </si>
+  <si>
+    <t>In [function] : Missing values in x, omitting rows</t>
+  </si>
+  <si>
+    <t>This is a warning rather than an error - some of the data has missing rows, so the function is just going to omit them from calculations.</t>
+  </si>
+  <si>
+    <t>reached getOption("max.print") -- omitted 384 rows</t>
+  </si>
+  <si>
+    <t>reached getOption("max.print") -- omitted x rows</t>
+  </si>
+  <si>
+    <t>Not an error: R will only print out so much data before deciding that you've had enough. This is the "max.print" option referenced. You can change this if you need to.</t>
+  </si>
+  <si>
+    <t>Error: as_tsibble doesn't know how to deal with this type of class yet.</t>
+  </si>
+  <si>
+    <t>Error: [packages] doesn't know how to deal with this type of class</t>
+  </si>
+  <si>
+    <t>Bespoke warning specifically from the tsibble package - you've passed the function an object in a format it doesn't know how to cope with. Try transforming the object as away around this. One way to work out solutions is to check vignettes and the package site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> comparison (1) is possible only for atomic and list types</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> comparison is possible only for atomic and list types</t>
+  </si>
+  <si>
+    <t>You just tried to do something that's only possible for data structures that are either atomic or lists. This is only helpful if you know what those  are! For a quick and basic rundown on atomic and lists see here: http://rex-analytics.com/r-for-excel-users/ For detailed information see here: http://adv-r.had.co.nz/Data-structures.html</t>
+  </si>
+  <si>
+    <t>Error in wf(.) : could not find function "wf"</t>
+  </si>
+  <si>
+    <t>Error in x(.) : could not find function "x"</t>
+  </si>
+  <si>
+    <t>A couple of things may have gone wrong here. Are you trying to call a function or did you think you were referring to a variable? If you were trying to call a function start by thinking about two things: is it spelled correctly? Is the package it comes from installed? If you tried to call a variable: did you put it in the right place? Is R expecting a function there instead? (This is a common mistake in a ggplot2 call.)</t>
+  </si>
+  <si>
+    <t>missing value where TRUE/FALSE needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The function went looking for a boolean (TRUE/FALSE) and got a big fat nothing, couldn't cope with it and aborted. </t>
+  </si>
+  <si>
+    <t>Error in bestFit[index[j], 1] : subscript out of bounds</t>
+  </si>
+  <si>
+    <t>Error in x[dim1, dim2]: subscript out of bounds</t>
+  </si>
+  <si>
+    <t>This error is typically when you have attempted to reference a part of an object using the [] notation. There are a few things that could have gone wrong. You could have used a dimension which is too big - beyond the length or width of the object, e.g. you could have gone looking for x[5] when x only has a length of 3. Or you could be using a dimension that doesn't exist for that object - referencing a vector with [n,1] often won't work because a vector typically has one dimension - so [n] would be the correct subscript. Or you might be referencing a matrix with one dimension when you need two - or an array and so on. Working out which is which can be quite hard. Use commands like dim() to find the dimensions - if this returns an error, you probably have a vector. length(), nrow() and ncol() are also very helpful, as well as str().</t>
+  </si>
+  <si>
+    <t>Error in names(x) &lt;- value :   'names' attribute [4] must be the same length as the vector [3]</t>
+  </si>
+  <si>
+    <t>Error in names(x) &lt;- value :   'names' attribute [a] must be the same length as the vector [b]</t>
+  </si>
+  <si>
+    <t>You just tried to name something, but either gave it too many or not enough names. If you check the length of your names vector and the dimension you're trying to name of your object with nrow() or ncol() this should fix that right up.</t>
+  </si>
+  <si>
+    <t>Error in `[&lt;-.data.frame`(`*tmp*`, index[j], value = "ann") :   new columns would leave holes after existing columns</t>
+  </si>
+  <si>
+    <t>new columns would leave holes after existing columns</t>
+  </si>
+  <si>
+    <t>This is obscure. It looks like you're trying to insert something into a data structure that already exists, but it's not a good 'shape'. When I've had this before, I've actually been accessing the wrong dimensions of objects (not including all relevant dimensions). This StackOverflow question appears to deal with a similar issue: https://stackoverflow.com/questions/43334695/r-error-new-column-would-leave-holes-after-existing-columns</t>
+  </si>
+  <si>
+    <t>In runif(1, min = 1, max = (nrow(modelList) + 1)) : NAs produced</t>
+  </si>
+  <si>
+    <t>In runif(1, min, max ) : NAs produced</t>
+  </si>
+  <si>
+    <t>A warning rather than an error, you're trying to produce random uniform variates, but the settings you've used are producing some missing data - chances are the min or max you've set is incorrect, or the length of the object to be produced is weird. If you're using variables as arguments in this function, this is probably where the problems stems from.</t>
+  </si>
+  <si>
+    <t>Error in nnetar(estY) : Not enough data to fit a model</t>
+  </si>
+  <si>
+    <t>Error in function(x) : Not enough data to fit a model</t>
+  </si>
+  <si>
+    <t>You're attempting to model something, but you just don't have enough data. A common problem, this can mean too many variables in a regression or regression-like model compared to your data. Some good discussion on that here: https://quant.stackexchange.com/questions/1664/how-many-explanatory-variables-is-too-many</t>
+  </si>
+  <si>
+    <t>Error in null.space.dimension() :   argument "d" is missing, with no default</t>
+  </si>
+  <si>
+    <t>Error in function(): argument "x" is missing with no default</t>
+  </si>
+  <si>
+    <t>You're missing an argument to the function you just tried to call. Sometimes functions have arguments with default values - if you don't fill them in, the function has a default it uses instead. This one doesn't have a default for this function so R has had a conniption. Sorry about that.</t>
+  </si>
+  <si>
+    <t>In chartData$time &lt;- seq(1, numGen, 1) : Coercing LHS to a list</t>
+  </si>
+  <si>
+    <t>In function: coercing LHS to a list</t>
+  </si>
+  <si>
+    <t>This is a warning not a function - you gave R a non-list object like a dataframe, but in order to complete the function, it must 'coerce' the object to a list. That is, it's changing the object type. This may be OK, or it may cause you some problems - either way, now you know! You can use functions like as.vector() or as.matrix() or as.data.frame() to change the object back from the list, but depending on the structure of your problem, that may not work alone. Sometimes it's easier to create an intermediary variable like this: (1) temp &lt;- function(x), (2) temp &lt;- as.data.frame(temp) 3) do whatever it is you wanted to do. That may not work for your problem, but it's worked for a few of mine!</t>
+  </si>
+  <si>
+    <t>Error in x[[jj]][iseq] &lt;- vjj :  incompatible types (from closure to logical) in subassignment type fix</t>
+  </si>
+  <si>
+    <t>Uh… yeah that's a pretty obscure one. Basically, R was expecting a variable not a function in there somewhere and didn't know what to do with what you gave it. This is an error that comes up sometimes when you're trying to write a closure (a function that builds other functions) and have gotten it wrong.</t>
+  </si>
+  <si>
+    <t>Error in as.character(choiceModel) :   cannot coerce type 'closure' to vector of type 'character'</t>
+  </si>
+  <si>
+    <t>Error in function():   cannot coerce type TYPE1 to vector of type TYPE2</t>
+  </si>
+  <si>
+    <t>In order to complete the operation, R needs at least one of the inputs into this function to be of the second type, whatever that is. It might be logical, integer, numeric, character - you get the drift. Currently, the critical input is of a different type and R can't coerce (meaning, convert in this case) that object to be the right type. So it's up to you to work out how to do that! Your steps: Which of the inputs into the function is causing the issue? What is its current type? What is the type it needs to be? Often simple fixes like as.data.frame() or as.numeric() or any of the as.[insert thing here]() function family work quite well here.</t>
+  </si>
+  <si>
+    <t>Error in accuracy(modelList[[choiceModel]](estY, ...)) :   '...' used in an incorrect context</t>
+  </si>
+  <si>
+    <t>Error in function(x): '…' used in an incorrect context</t>
+  </si>
+  <si>
+    <t>The '…' notation in R is a very powerful tool that allows programmers to pass an arbitrary number of arguments (inputs) into a function. It's great! But it requires some skill to use and R didn't like how you used it here. Pro tip: when searching for info search for "three dots ellipsis" not "..." because it will produce much better results. https://ipub.com/r-three-dots-ellipsis/</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>The three dot ellipsis: trust me you want to search for this term, not "…" in google! This is a method for passing arbitrary numbers of arguments into and out of functions in R. You can read more about it here: https://ipub.com/r-three-dots-ellipsis/</t>
+  </si>
+  <si>
+    <t>Error in vector(NA, length = length(modelList)) :   vector: cannot make a vector of mode 'NA'.</t>
+  </si>
+  <si>
+    <t>It looks like you accidentally got the order or type of arguments to this function incorrect here. Try ?functionName or ??functionName for more information about this function</t>
+  </si>
+  <si>
+    <t>Error in modelList[[choiceModel]](estY, h) : unused argument (h)</t>
+  </si>
+  <si>
+    <t>Error in function : unused argument (x)</t>
+  </si>
+  <si>
+    <t>You've added an extra argument to this function is not required. R gets confused and wants you to remove it.</t>
+  </si>
+  <si>
+    <t>Error in value[[3L]](cond) : unused argument (cond)</t>
+  </si>
+  <si>
+    <t>Error in function() : unused argument (cond)</t>
+  </si>
+  <si>
+    <t>This probably refers to errors in a tryCatch() statement you may have in your code - do you have an empty function within the tryCatch statement?. Further information here https://github.com/aryoda/tryCatchLog/issues/17 and here: https://stackoverflow.com/questions/31854304/what-is-error-in-value3lcond-in-r</t>
+  </si>
+  <si>
+    <t>Error in estY[1] + 10000 : non-numeric argument to binary operator</t>
+  </si>
+  <si>
+    <t>Error in function() : non-numeric argument to binary operator</t>
+  </si>
+  <si>
+    <t>Some discussion here: http://www.dummies.com/programming/r/how-to-read-errors-and-warnings-in-r/ you used an argument that is not a number in conjunction with an operator (e.g. + or -) that needs numeric input. For example, "cat" + "dog" doesn't make sense in R the same way that 3 + 4 would.</t>
+  </si>
+  <si>
+    <t>Error: attempt to use zero-length variable name</t>
+  </si>
+  <si>
+    <t>Names, by definition have to have something in them! You may have made a mistake in your typing or in your code somewhere, but you tried to name something nothing.</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>SDS</t>
+  </si>
+  <si>
+    <t>Attempt at Common/General Form</t>
+  </si>
+  <si>
+    <t>Error in install.packages : object 'tidyverse' not found</t>
+  </si>
+  <si>
+    <t>Error in install.packages : object x not found</t>
+  </si>
+  <si>
+    <t>install.packages() can fail for a few reasons, but the most common are: did you spell the package name correctly and/pr did you put the name in inverted commas: "packageName"? If you did both of these things, is the package actually on CRAN or somewhere else? To find out if the package is on CRAN, you can search for it here: https://cran.r-project.org/web/packages/available_packages_by_name.html (pro tip: go to edit/find/find on page in your browser - there's a huge number of packages to wade through) If it's not on CRAN then you will need to install this package from another source. Check where the package is hosted - the package developer will usually have documentation telling you if it's on Github, Bioconductor or some other hosting method.</t>
+  </si>
+  <si>
+    <t>Error: object 'mgp' not found</t>
+  </si>
+  <si>
+    <t>Error: object x not found</t>
+  </si>
+  <si>
+    <t>R couldn't find this 'object'. An object is just code-speak for some kind of construct - that can be a data frame, a document, a function, a chart or any one of a number of things. There are a few reasons why objects can't be found by R: you  may not have named it correctly - did you spell it right? You may have R to look for it in the wrong place - is your working directory where you intended it to be? If you work in R Studio, most working directory-related problems can be solved using projects, see here for details: http://stat545.com/block002_hello-r-workspace-wd-project.html Lastly, have you defined the object (commonly a variable or function when you start out!) before you tried to use it? You'd be surprised how often this is an issue!</t>
+  </si>
+  <si>
+    <t>mapping: x = displ, y = hwy 
+geom_point: na.rm = FALSE
+stat_identity: na.rm = FALSE
+position_identity</t>
+  </si>
+  <si>
+    <t>Error in ggplot(data = xyz) : object 'xyz' not found</t>
+  </si>
+  <si>
+    <t>Error in FUN(X[[i]], ...) : object 'display' not found</t>
+  </si>
+  <si>
+    <t>Error: geom_point requires the following missing aesthetics: x, y</t>
+  </si>
+  <si>
+    <t>This one is caused when you call ggplot2 to create a chart, but as you add layers you forgot to add a + at the end of the previous layer, for example: ggplot(data = mpg) 
+  geom_point(mapping = aes(x = displ, y = hwy)) this is solved by adding a + after ggplot(data = mpg). It should be after the first line and NOT before the second line, e.g. NOT as +geom_point(mapping = aes(x = displ, y = hwy)) because this makes R very sad. For ggplot2 help see here: http://ggplot2.org/book/</t>
+  </si>
+  <si>
+    <t>ggplot doesn't know where to find the data you've told it it plot. For ggplot2 help see here: http://ggplot2.org/book/</t>
+  </si>
+  <si>
+    <t>ggplot(data = mpg) +   geom_point(mapping = aes(x = display, y = hwy)) in this error, ggplot didn't understand which part of the data frame to put on the x axis, because the name it references is spelt incorrectly. For ggplot2 help see here: http://ggplot2.org/book/</t>
+  </si>
+  <si>
+    <t>Did you include a statement with aes(x = …, y = …) somewhere in your ggplot call? Ggplot needs to understand HOW to build up the layers and to map the dataframe into a visual representation and without the aes() statement, it just doesn't know how. For ggplot2 help see here: http://ggplot2.org/book/</t>
+  </si>
+  <si>
+    <t>Error: geom_line requires the following missing aesthetics: y</t>
+  </si>
+  <si>
+    <t>A line chart is essentially a mapping between two variables: but you've only given ggplot one to work with, so it needs the other! If you want a line chart of the count of a single variable or something like that, then this is a little more complex. geom_bar() is the simplest method and for some details see here: http://r4ds.had.co.nz/data-visualisation.html#statistical-transformations</t>
+  </si>
+  <si>
+    <t>Error: stat_count() must not be used with a y aesthetic.</t>
+  </si>
+  <si>
+    <t>You're using a ggplot geom which needs the function stat_count(). This is probably geom_bar() if you're just starting out. However, you passed it a second argument to the aes() mapping, e.g. a y variable when you already had an x variable. This is a problem because in the case of this geom, it's a univariate process and it doesn't know what to do with a second variable. Have you got the right geom for the chart you're trying to produce? It's always a good idea to draw a mock up of what you want to produce and then work backwards to see which mappings and data structures will get you there. For more ggplot2 help see here: http://r4ds.had.co.nz/data-visualisation.html#statistical-transformations</t>
+  </si>
+  <si>
+    <t>Error: Expected at least one column name; e.g. `~name`</t>
+  </si>
+  <si>
+    <t>Are you trying to load a tribble or tibble directly into the console? Do all the column names have ~ in front of them? This sort of error will give you this message. For further help on tribbles and tibbles, see here: http://r4ds.had.co.nz/tibbles.html</t>
+  </si>
+  <si>
+    <t>Error in if (is.waive(data) || empty(data)) return(cbind(data, PANEL = integer(0))) :   missing value where TRUE/FALSE needed</t>
+  </si>
+  <si>
+    <t>Code that threw the error</t>
+  </si>
+  <si>
+    <t>install.packages(tidyverse)</t>
+  </si>
+  <si>
+    <t>mgp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt; ggplot(data = mpg)  &gt;   geom_point(mapping = aes(x = displ, y = hwy)) </t>
+  </si>
+  <si>
+    <t>ggplot(data = xyz) +
++   geom_point(mapping = aes(x = displ, y = hwy))</t>
+  </si>
+  <si>
+    <t>ggplot(data = mpg) +
++   geom_point(mapping = aes(x = display, y = hwy))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ggplot(mpg) +
++   geom_point()</t>
+  </si>
+  <si>
+    <t>ggplot(data = diamonds) + 
++   geom_line(aes(x = cut))</t>
+  </si>
+  <si>
+    <t>ggplot(data = diamonds) + 
++   geom_bar(aes(x = cut, y = clarity))</t>
+  </si>
+  <si>
+    <t>demo &lt;- tribble(
++   cut,         ~freq,
++   "Fair",       1610,
++   "Good",       4906,
++   "Very Good",  12082,
++   "Premium",    13791,
++   "Ideal",      21551
++ )</t>
+  </si>
+  <si>
+    <t>ggplot(data = demo) +
++   geom_bar(mapping = aes(x = cut, y = freq))</t>
+  </si>
+  <si>
+    <t>This one has me really stumped, to be honest. Correct code should have been: ggplot(data = demo) +
+  geom_bar(mapping = aes(x = cut, y = freq), stat = "identity") I THOUGHT I would have gotten an error similar to stat_count() must not be used with a y aesthetic.</t>
+  </si>
+  <si>
+    <t>ggplot(data = diamonds) + 
++     geom_bar(mapping = aes(x = cut, y = ..prop.))</t>
+  </si>
+  <si>
+    <t>Error in FUN(X[[i]], ...) : object '..prop.' not found</t>
+  </si>
+  <si>
+    <t>The ..prop.. Function is incorrectly called here, spelling error. This is a fairly common type of error when you can't type.</t>
+  </si>
+  <si>
+    <t>ggplot(data = diamonds, mapping = aes(x = cut, fill = clarity)) + 
++   geom_bar(alpha = 1/5, position = identity)</t>
+  </si>
+  <si>
+    <t>Error in self$position$setup_params : 
+  object of type 'closure' is not subsettable</t>
+  </si>
+  <si>
+    <t>This is a strange one for ggplot. Object of type 'closure' is not subsettable simply means that R doesn't know how to take slices out of a function definition. Which is fair enough, I don't know how to take them either. In a ggplot2 context, this error occurs when position calls are used incorrectly. I expected an 'object not found' error (the problem here is that identity is not enclosed by quote marks: "identity").</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggplot(data = diamonds) + 
+  geom_bar(mapping = aes(x = cut, fill = clarity), position = dodge)
+</t>
+  </si>
+  <si>
+    <t>Error in layer(data = data, mapping = mapping, stat = stat, geom = GeomBar,  : 
+  object 'dodge' not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here, the error tells you which layer of the chart caused the problem and which object could not be found. </t>
+  </si>
+  <si>
+    <t>ggplot(data = mpg) + 
+  geom_point(mapping = aes(x = displ, y = hwy), position = jitter)</t>
+  </si>
+  <si>
+    <t>ggplot(data = mpg, mapping = aes(x = class, y = hwy)) + 
+  geom_boxplot() +
+  cord_flip()</t>
+  </si>
+  <si>
+    <t>Error in cord_flip() : could not find function "cord_flip"</t>
+  </si>
+  <si>
+    <t>Have you spelled the function call correctly?</t>
+  </si>
+  <si>
+    <t>Error in functionName(): could not find function "functionName"</t>
+  </si>
+  <si>
+    <t>filter(flights, month = 1, day == 1)</t>
+  </si>
+  <si>
+    <t>Error: `month` (`month = 1`) must not be named, do you need `==`?</t>
+  </si>
+  <si>
+    <t>The real clue here is in the 'do you need `==`?' In dplyr::filter you're trying to use regular assignment (=) instead of a strong assignment (==).</t>
+  </si>
+  <si>
+    <t>Error: `x` (`x = a`) must not be named, do you need `==`?</t>
+  </si>
+  <si>
+    <t>Error in filter(fligts, month == 1, day == 1) : object 'fligts' not found</t>
+  </si>
+  <si>
+    <t>R could not find the object that filter should be working on - did you spell it correctly? Is it loaded into memory?</t>
+  </si>
+  <si>
+    <t>arrange(flights, x, month, day)</t>
+  </si>
+  <si>
+    <t>Error in arrange_impl(.data, dots) : 
+  Evaluation error: object 'x' not found.</t>
+  </si>
+  <si>
+    <t>select(flights, x, month, day)</t>
+  </si>
+  <si>
+    <t>Error in overscope_eval_next(overscope, expr) : object 'x' not found</t>
+  </si>
+  <si>
+    <t>Object not found means that one of the items you're attempting to work on is not in the data frame you specified (or that the data frame itself may not be available) - have you had a misspelling or is the data all in the one data frame?</t>
+  </si>
+  <si>
+    <t>select(flight, year, month, day)</t>
+  </si>
+  <si>
+    <t>Error in select(flight, year, month, day) : object 'flight' not found</t>
+  </si>
+  <si>
+    <t>rename(flights, tail_num = tailnumzzz)</t>
+  </si>
+  <si>
+    <t>Error: `tailnumzzz` contains unknown variables</t>
+  </si>
+  <si>
+    <t>The varaiable you are attempting to rename is unrecognised by R. Have you spelt it correctly or is it in the data frame you specified?</t>
+  </si>
+  <si>
+    <t>mutate(flights,
+       gain = arr_delay - dep_delay,
+       speed = distancezzz / air_time * 60
+)</t>
+  </si>
+  <si>
+    <t>Error in mutate_impl(.data, dots) : 
+  Evaluation error: object 'distancezzz' not found.</t>
+  </si>
+  <si>
+    <t>This is a strange one for ggplot. Object of type 'closure' is not subsettable simply means that R doesn't know how to take slices out of a function definition. Which is fair enough, I don't know how to take them either. In a ggplot2 context, this error occurs when position calls are used incorrectly. I expected an 'object not found' error (the problem here is that jitter is not enclosed by quote marks: "jitter").</t>
+  </si>
+  <si>
+    <t>One of the variables you are attempting to manipulate is not recognisable as part of the data frame you called - it is spelled correctly and is it in the dataframe you specified?</t>
+  </si>
+  <si>
+    <t>delays &lt;- flights %&gt;% 
+  group_by(dest)
+%&gt;%  summarise(
+    count = n(),
+    dist = mean(distance, na.rm = TRUE),
+    delay = mean(arr_delay, na.rm = TRUE)
+  ) %&gt;% 
+  filter(count &gt; 20, dest != "HNL")</t>
+  </si>
+  <si>
+    <t>Error: unexpected SPECIAL in "%&gt;%"</t>
+  </si>
+  <si>
+    <t>Did the pipe (%&gt;%) go at the end of the line? If it's not placed correctly it throws weird errors! It should go at the end of the line like the + in ggplot2 layers.</t>
+  </si>
+  <si>
+    <t>Error: unexpected symbol in:
+"    count = n()
+    dist"</t>
+  </si>
+  <si>
+    <t>unexpected symbol</t>
+  </si>
+  <si>
+    <t>This sort of error typically occurs when R hit a piece of punctuation or a symbol in a place it didn't expect. Do you have missing commas or an extra one? Do you have unmatched brackets somewhere? This is a common sort of problem you'll encounter with this error. It can also be hard to spot! If you are working in RStudio there are some tools built into the script editor to help you: look for red crosses down the left hand side, they will tell you where some of the problems lie. If you place the cursor just behind a bracket, it will automatically highlight its matching pair. This will help you understand what area of code they enclose. Remember that brackets have to be matched - (} won't work, [) won't either! They mean different things and belong in matched pairs.</t>
+  </si>
+  <si>
+    <t>delays &lt;- flights %&gt;% 
+  group_by(dest) %&gt;%
+  summarise(
+    count = n()
+    dist = mean(distance, na.rm = TRUE),
+    delay = mean(arr_delay, na.rm = TRUE)
+  ) %&gt;% 
+  filter(count &gt; 20, dest != "HNL")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flights %&gt;% 
+  group_by(year, month, day) %&gt;% 
+  summarise(mean = meanzzz(dep_delay))
+</t>
+  </si>
+  <si>
+    <t>Error in summarise_impl(.data, dots) : 
+  Evaluation error: could not find function "meanzzz".</t>
+  </si>
+  <si>
+    <t>The "could not find function" is the clue here - have you spelt the function call correctly? Is the package the function belongs to loaded? (E.g. have you run the code library(packageName)?) If you are unsure which package the function belongs to, try ?functionName or ??functionName. Alternatively, https://www.rdocumentation.org is a good place to search.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not_cancelled &lt;- flights %&lt;%
+  filter(!is.na(dep_delay), !is.na(arr_delay))
+</t>
+  </si>
+  <si>
+    <t>Error in flights %&lt;% filter(!is.na(dep_delay), !is.na(arr_delay)) : 
+  could not find function "%&lt;%"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ggplot(data = delays, mapping = aes(x = delay)) + 
+  geom_freqpoly(binwidth = x)
+</t>
+  </si>
+  <si>
+    <t>Error in geom_freqpoly(binwidth = x) : object 'x' not found</t>
+  </si>
+  <si>
+    <t>Object not found means that one of the items you're attempting to work on is not where it thought it should be. Have you had a misspelling, or is a variable not been defined yet?</t>
+  </si>
+  <si>
+    <r>
+      <t>batting &lt;-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color rgb="FF4070A0"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9.35"/>
+        <color rgb="FF007020"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>as_tibble</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.35"/>
+        <color rgb="FF333333"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t>(Lahman::Batting)</t>
+    </r>
+  </si>
+  <si>
+    <t>Error in loadNamespace(name) : there is no package called ‘Lahman’</t>
+  </si>
+  <si>
+    <t>In its simplest form, this is another way of saying that the package you've referenced is not on your computer.You'll need to use install.packages() or another method of obtaining the relevant package.</t>
+  </si>
+  <si>
+    <t>not_cancelled %&gt;% 
+  group_by(year, month, day) %&gt;% 
+  summarise(
+    avg_delay1 = mean(arr_delay),
+    avg_delay2 = mean(arr_delay[arr_delay &gt; 0) # the average positive delay
+  )</t>
+  </si>
+  <si>
+    <t>Error: unexpected ')' in:
+"    avg_delay1 = mean(arr_delay),
+    avg_delay2 = mean(arr_delay[arr_delay &gt; 0)"</t>
+  </si>
+  <si>
+    <t>not_cancelled %&gt;% 
+  group_by(dest) %&gt;% 
+  summarise(distance_sd == sd(distance)) %&gt;% 
+  arrange(desc(distance_sd))</t>
+  </si>
+  <si>
+    <t>Error in summarise_impl(.data, dots) : 
+  Evaluation error: object 'distance_sd' not found.</t>
+  </si>
+  <si>
+    <t>Object not found typically means a spelling error or an undefined object - if you think the object should be defined in the command that's causing the error - is it possibile you've used a comparative operator (for e.g. ==) instead of an assignment operator (&lt;- or =). The difference between comparison and assignment in R is reserved for specific operators so comparison operators return a boolean outcome -TRUE or FALSE. Assignment operators act more like the classic equals - cat &lt;- 5 or dog = 10 will give you new variables equalling 5 or 10 respectively.</t>
+  </si>
+  <si>
+    <t>Error in read.xlsx.default("database.xlsx", sheet = "troubleshooting",  : 
+  File does not exist.</t>
+  </si>
+  <si>
+    <t>troubleShootDB &lt;- read.xlsx("database.xlsx", sheet = "troubleshooting",
++                             colNames = TRUE)</t>
+  </si>
+  <si>
+    <t>Are you certain the file is located where you think it is or have you misspelled the file name? Sometimes when we are working in a different directory, the path that R uses to find the file can get confusing. Try using getwd() to find out where you are. Projects are also a good way of avoiding some of these issues in RStudio. A good discussion of projects can be found here: https://www.tidyverse.org/articles/2017/12/workflow-vs-script/</t>
+  </si>
+  <si>
+    <t>devtools::use_data(defineDB)</t>
+  </si>
+  <si>
+    <t>Error: defineDB.rda already exists in /Users/Steph/Documents/Rex Analytics/Blog/Excel users/helpPlease/data. Use overwrite = TRUE to overwrite</t>
+  </si>
+  <si>
+    <t>You're about to replace a file in your package: are you really sure you want to do that? If so, use command as suggested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in sheets_fun(path) : 
+  zip file 'raw-data/database.xlsx' cannot be opened
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db &lt;- read_xlsx("raw-data/database.xlsx", sheet = "helpError",
+                col_names = TRUE) %&gt;%
+          as.data.frame()
+</t>
+  </si>
+  <si>
+    <t>Error in readRDS(defineDB) : bad 'file' argument</t>
+  </si>
+  <si>
+    <t>R cannot find your file!</t>
+  </si>
+  <si>
+    <t>aesthetic</t>
+  </si>
+  <si>
+    <t>binary</t>
+  </si>
+  <si>
+    <t>binwidth</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>coerce</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>geom</t>
+  </si>
+  <si>
+    <t>library</t>
+  </si>
+  <si>
+    <t>na.rm</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>subsettable</t>
+  </si>
+  <si>
+    <t>In the context of ggplot, an aesthetic is how the grammar of graphics maps the data into a visual format. See here: http://ggplot2.tidyverse.org/reference/aes.html</t>
+  </si>
+  <si>
+    <t>An argument is an input into a function. Some functions take no arguments encouragement() is one of those. The brackets are still needed after the name, however, because they tell R to go look for a function, not a variable. Most functions take one or more arguments, for example in mean(x) the argument is x.</t>
+  </si>
+  <si>
+    <t>Typically this is an object with one of two options. Sometimes coded 0 and 1, TRUE and FALSE etc.</t>
+  </si>
+  <si>
+    <t>Binwidth is the width of the bars in a histogram. Choosing the 'right' binwidth can be quite complicated and you will almost always want to try a few different ones to see what fits your data best. There are lots of automated 'rules' for choosing binwidths out there in stats, but they should be thought of as a starting point only.</t>
+  </si>
+  <si>
+    <t>Character is a type of data in R. It just means that the data is not considered to have numerical properties attached to it. Characters should be enclosed in "quotes" so R knows it's not looking for a variable by that name.</t>
+  </si>
+  <si>
+    <t>Class is a structure used in object oriented programming. To find out more about it, check this out: https://www.rdocumentation.org/packages/base/versions/3.4.3/topics/class</t>
+  </si>
+  <si>
+    <t>Coerce is a nice way of saying "R is going to try and force your objects to do something. It may or may not work."</t>
+  </si>
+  <si>
+    <t>A function is a way of taking a block of code and using it to do a whole bunch of things, many times. Well worth the effort to learn how to build your own - check this out: https://www.stat.berkeley.edu/~statcur/Workshop2/Presentations/functions.pdf</t>
+  </si>
+  <si>
+    <t>A geom is how ggplot2 maps data into a visual format. Obviously it's more complex than that, but this page is a good rundown of the basics: http://ggplot2.tidyverse.org/reference/</t>
+  </si>
+  <si>
+    <t>The package library is where all the packages you installed on your computer (e.g. ggplot, dplyr etc.) lives.</t>
+  </si>
+  <si>
+    <t>R's missing value coding</t>
+  </si>
+  <si>
+    <t>na.rm is a fairly common shorthand in a lot of functions. It means "remove missing values" and takes one of two options- TRUE or FALSE</t>
+  </si>
+  <si>
+    <t>Subsetting is the practice of taking slices out of an object. For example, if I have a matrix called X that is 100 x 100, I can subset that matrix by taking only the first ten rows and the fifth column. In R that would look like X[1:10,5]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,6 +839,22 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.35"/>
+      <color rgb="FF333333"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.35"/>
+      <color rgb="FF007020"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <sz val="9.35"/>
+      <color rgb="FF4070A0"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,13 +877,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,97 +1184,850 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" customWidth="1"/>
-    <col min="3" max="3" width="101.1640625" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="43.6640625" customWidth="1"/>
+    <col min="4" max="4" width="101.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="C1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="150" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="150" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="120" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>149</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="75" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="120" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+      <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="60" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C37" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D38" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="E38" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D39" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D40" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C41" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D41" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
         <v>37</v>
       </c>
+      <c r="D42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C56" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" t="s">
+        <v>84</v>
+      </c>
+      <c r="D58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
+      <c r="D59" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D63">
+    <sortCondition ref="A2:A63"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -584,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -597,18 +2048,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -616,15 +2067,15 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -632,7 +2083,119 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -652,26 +2215,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -691,26 +2254,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>